<commit_message>
Adding new testcase for booking appointment
</commit_message>
<xml_diff>
--- a/GoHighLevelTestProject/UseCase.xlsx
+++ b/GoHighLevelTestProject/UseCase.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sagportal-my.sharepoint.com/personal/shek_softwareag_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{28AE4C13-FFF6-45B0-A703-BA4ACC9E1B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3FF83E9-C271-497C-9E26-EE05B2FE74B8}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{61C27527-D8E0-41F1-9C4B-EA4FFBCC30B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E85A3C1A-B73C-4B55-8D5A-DD52591C2283}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03B1D8C8-E9F4-4F96-9C00-C1FF27208331}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{03B1D8C8-E9F4-4F96-9C00-C1FF27208331}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimize Appointment" sheetId="1" r:id="rId1"/>
     <sheet name="Appointment per day and slot" sheetId="2" r:id="rId2"/>
-    <sheet name="Booking Widget" sheetId="3" r:id="rId3"/>
-    <sheet name="Calendar Configuration" sheetId="4" r:id="rId4"/>
+    <sheet name="Calendar Configuration" sheetId="4" r:id="rId3"/>
+    <sheet name="TimeZone" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that edit calendar page is opening up after clicking on edit from ellipsis </t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -59,51 +53,24 @@
     <t>When number of appointment per day is 1</t>
   </si>
   <si>
-    <t>Verify that all the members are selected by default</t>
-  </si>
-  <si>
-    <t>Verify priority dropdown is coming infront of all members</t>
-  </si>
-  <si>
     <t>Verify that member with high priority gets the appointment</t>
   </si>
   <si>
     <t>Verify that  member with low priority shouldnot get the appointment</t>
   </si>
   <si>
-    <t>Verify that all the members in the team is coming up for optimize availability</t>
-  </si>
-  <si>
-    <t>Verify that all the members in the team is coming up for optimize for equal distribution</t>
-  </si>
-  <si>
     <t>Verify that appointment should be allocated for any of the high priority members if more than one member with high priority is selected</t>
   </si>
   <si>
-    <t>Verify that member with low priority shouldnot get the appointment</t>
-  </si>
-  <si>
     <t>Verify unselected team member should not get the appointment</t>
   </si>
   <si>
     <t>Optimize for Equal distribution</t>
   </si>
   <si>
-    <t>Verify priority dropdown is not coming for team members</t>
-  </si>
-  <si>
-    <t>Verify that any of the team member is getting allocated for the first appointment(assumption tester1 got the appointment)</t>
-  </si>
-  <si>
-    <t>Verify that any of the team member except(tester1) the one allocated in above usecase is getting allocated for the next appointment booked</t>
-  </si>
-  <si>
     <t>Verify user is able to book appointment for the day not booked by others</t>
   </si>
   <si>
-    <t>Verify any of the  selected team member should get the appointment</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user or member is not able to book appointment if other user booked for the same date </t>
   </si>
   <si>
@@ -119,40 +86,10 @@
     <t>Verify that user or member is not able to book appointment for same date once appointment is already booked</t>
   </si>
   <si>
-    <t>Verify user is able to book appointment for the day not booked by others(e.g 1stmarch,8am)</t>
-  </si>
-  <si>
-    <t>Verify second appointment can be booked for the slot and date already booked by others, if team member is 3(e.g 1stmarch,8am)</t>
-  </si>
-  <si>
-    <t>Verify third appointment can be booked for the slot and date already booked by others, if team member is 3(e.g 1stmarch,8am)</t>
-  </si>
-  <si>
-    <t>Verify slot for the date not appearing when the slot and date already booked by others, if team member is 3(e.g 1stmarch,8am)</t>
-  </si>
-  <si>
-    <t>Verify second and third appointment can be booked for any other slot(e.g 1st march)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify second appointment gets allocated to any team members other than the one allocated in first appointment </t>
-  </si>
-  <si>
     <t>Verify that user or member sees the slot available for which the appointment is cancelled</t>
   </si>
   <si>
-    <t>Verify user is able to book appointment at the conflicting time (with another calendar) if any of the team member is available</t>
-  </si>
-  <si>
     <t>Verify particular slot is not visible for user to book appointment if none of the team members are available</t>
-  </si>
-  <si>
-    <t>Verify second appointment cannot be booked on the same date</t>
-  </si>
-  <si>
-    <t>Verify that user or member sees the slot available for the date which the appointment is cancelled</t>
-  </si>
-  <si>
-    <t>Creating new calendar with number of appointment per day is 1</t>
   </si>
   <si>
     <t>Verify for a new member, primary calendar is not selected</t>
@@ -226,7 +163,218 @@
     <t>Verify date is not available in configured calendar while booking appointment if in calendar all three users are selected or checked and appointment per day is 1</t>
   </si>
   <si>
-    <t>Automated</t>
+    <t>Step by Step description</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Booking Widget
+</t>
+  </si>
+  <si>
+    <t>User should be able to book meeting. User should be able to see booked meeting under calendars</t>
+  </si>
+  <si>
+    <t>User should be able to book appointment on the same date for which it was cancelled</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date(e.g. March 15th) should come up as disabled. User should not be able to book on same date booked by others.</t>
+  </si>
+  <si>
+    <t>date(e.g. March 15th) should come up as disabled. User should not be able to book on same date booked by others.</t>
+  </si>
+  <si>
+    <t>Teammembers(Tester2 and sheetal) shouldnot get the appointment as they are on low priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for availablilty" radiobutton
+3.Select Tester1 as High Priority
+and other two team members with low Priority
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 15th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for availablilty" radiobutton
+3.Select "Tester1" and "Tester2" as High Priority and other as Low Priority
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 15th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t>Either of the Teammember Tester1 or Tester 2 can get the appointment.
+Teammember sheetal should not get the appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for  availability" radiobutton
+3.Check all team members &gt; with same priority
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 15th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for Equal Distribution" radiobutton
+3.Select "Tester1", "Tester2" and "sheetal"
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 15th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t>Verify that any of the team member is getting allocated for the first appointment(Assumption tester1 got the appointment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for Equal Distribution" radiobutton
+3.Select "Tester1", "Tester2" and "sheetal"
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 16th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t>Any of the team member should get the appointment based on round robin fashin.
+Assumption is tester1 has got the appointment</t>
+  </si>
+  <si>
+    <t>Either of Tester2 or sheetal should get the appointment if their calendars are free for that date</t>
+  </si>
+  <si>
+    <t>Verify that any of the team member except(tester1) the one allocated in above usecase is getting allocated for the next appointment booked(if their calendars are free)</t>
+  </si>
+  <si>
+    <t>Appointment should be booked and assigned to either tester1 or sheetal. Appointment shouldnot be assigned to "Tester2"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on calendar settings
+2. Select "optimize for Equal Distribution" radiobutton
+3.Select "Tester1" and "sheetal" and uncheck "tester2"
+4. Click on Save
+5. Click on Booking Widget
+6. Click on date(e.g March 15th 11:30am)(Assumption no one has booked on this date)
+7.  Select time according to the team member availablility
+8. Enter basic information and schedule the meeting
+9. click on scheduling &gt; Appointments </t>
+  </si>
+  <si>
+    <t>Appointment should be booked and assigned to any of the team members</t>
+  </si>
+  <si>
+    <t>Appointment should be booked and Teammember(Tester1) should get the appointment as tester1 is on high priority</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget
+2. Click on date(e.g March 15th)(Assumption no one has booked on this date)
+3.  Select time according to the team member availablility e.g.9am
+4. Enter basic information and schedule the meeting
+5. click on scheduling &gt; appointment &gt; cancel created appointment
+6. Click on Booking widget
+7. select same date (e.g march 15th)
+8. select time according to the availability of team member
+9.click on scheduling&gt; calendar</t>
+  </si>
+  <si>
+    <t>Verify second appointment can be booked for the slot and date already booked by others, if team member is 3(e.g 15thmarch,9am)</t>
+  </si>
+  <si>
+    <t>Verify third appointment cannot be booked for the slot and date already booked by others, if team member is 3(e.g 15thmarch,9am)</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget
+2. Click on date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date(e.g. March 15th) should come up as disabled. User should not be able to book as two appointments are booked for the same date (e.g 15th march)</t>
+  </si>
+  <si>
+    <t>User should be able to book apoointment for the date and time alreay booked by another user(e.g 15thmarch 9am).</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget
+2. Click on date(e.g March 15th)(Assumption no one has booked on this date and members have marked their unavailability on that date)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date(e.g. March 15th) should come up as disabled. User shouldn’t be able to book appointment on that date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Booking Widget
+2. Click on date(e.g March 15th)(Assumption no one has booked on this date)
+3.  Select time according to the team member availablility (9a.m)
+4. Enter basic information and schedule the meeting
+5. click on scheduling &gt; calendar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Booking Widget
+2. Click on date(e.g March 15th)(Assumption first appointment has booked on this date and same time 9.am)
+3.  Select time according to the team member availablility (e.g 9am)
+4. Enter basic information and schedule the meeting
+5. click on scheduling &gt; calendar </t>
+  </si>
+  <si>
+    <t>GMT -7:00(America/Dawson)</t>
+  </si>
+  <si>
+    <t>Verify slots available to user in GMT-7:00 according to the service provider</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget
+2. Select date</t>
+  </si>
+  <si>
+    <t>UI(For understanding the usecase)</t>
+  </si>
+  <si>
+    <t>Verify user in different timezone able to book appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Booking Widget
+2. Click on date(e.g March 15th)(Assumption no one has booked on this date)
+3.  Select time according to the team member availablility (8p.m)
+4. Enter basic information and schedule the meeting
+5. click on scheduling &gt; calendar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment should be booked for service provider on 16th march at 9a.m </t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Verify user in different timezone not able to book appointment already booked by others on same date</t>
+  </si>
+  <si>
+    <t>1. Click on Booking Widget
+2. Click on date(e.g March 15th) where appointment is booked on others</t>
+  </si>
+  <si>
+    <t>Date 15th march should be disabled</t>
+  </si>
+  <si>
+    <t>Observe slots seen to user are from 7p.m -4a.m to user in calendar as service provider is in IST zone from 8a.m to 5pm</t>
   </si>
 </sst>
 </file>
@@ -282,13 +430,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,168 +757,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3310FED-7CD1-4168-B229-E766B9E67D09}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="107" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
+      <c r="C11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -774,208 +902,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA51D8E-6D39-41E2-B8B6-BA47613A2A1B}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:K1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="113.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="171.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2540B88-1D42-49DD-9A8D-CA1FCB3AE303}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="2" width="88.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3406B64D-F02E-4F5E-A482-87F4681B2828}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +1063,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1005,90 +1080,187 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402ACB70-7EB2-4954-9B4D-269BCD5CEC8C}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="55.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>